<commit_message>
class rename + xlsx  commit test
</commit_message>
<xml_diff>
--- a/RcOnline/base.xlsx
+++ b/RcOnline/base.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>Id</t>
   </si>
@@ -77,28 +77,19 @@
     <t>Не загружен справочник НСИ 16</t>
   </si>
   <si>
-    <t>Найдено 1 ЛС в ГИС ЖКХ (обл Свердловская,г Сухой Лог,ул Артиллеристов,28)</t>
-  </si>
-  <si>
-    <t>Не найден аккаунт для кап. ремонта в ГИС ЖКХ</t>
+    <t>Найдено 0 ПУ в ГИС ЖКХ (обл Свердловская,г Сухой Лог,ул Рябиновая,20)</t>
   </si>
   <si>
     <t>Не загружен справочник НСИ 50 (Жил. услуги)</t>
   </si>
   <si>
-    <t>Выполняю выгрузку начислений в ГИС ЖКХ для компании ООО "Белокалитвинская УК"</t>
-  </si>
-  <si>
-    <t>Найдено 0 ЛС в ГИС ЖКХ (обл Свердловская,г Заречный,ул Ленинградская,12А)</t>
+    <t>ПД выгружен успешно</t>
   </si>
   <si>
     <t>Выполняю выгрузку начислений в ГИС ЖКХ для компании ТСЖ "Спортивная 7"</t>
   </si>
   <si>
-    <t>Выполняю выгрузку начислений в ГИС ЖКХ для компании МУП "ГУЖКХ"</t>
-  </si>
-  <si>
-    <t>Выполняю выгрузку начислений в ГИС ЖКХ для компании ООО УК Жилфонд</t>
+    <t>Не найдены услуги в ГИС ЖКХ: 'Вывоз ЖБО, ТБО'</t>
   </si>
   <si>
     <t>Компания</t>
@@ -391,7 +382,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="16">
+  <numFmts count="20">
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="0" formatCode="General"/>
@@ -500,33 +495,33 @@
   <sheetData>
     <row r="1" ht="12.8" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" ht="12.8">
       <c r="A2" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D2" s="7">
         <v>441</v>
@@ -540,13 +535,13 @@
     </row>
     <row r="3" ht="12.8">
       <c r="A3" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D3" s="7">
         <v>444</v>
@@ -560,13 +555,13 @@
     </row>
     <row r="4" ht="12.8">
       <c r="A4" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D4" s="7">
         <v>445</v>
@@ -574,7 +569,7 @@
     </row>
     <row r="5" ht="12.8">
       <c r="A5" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" s="7">
         <v>1116674008098</v>
@@ -594,7 +589,7 @@
     </row>
     <row r="6" ht="12.8">
       <c r="A6" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" s="7">
         <v>1047405001049</v>
@@ -611,7 +606,7 @@
     </row>
     <row r="7" ht="23.95">
       <c r="A7" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" s="7">
         <v>5117401000129</v>
@@ -631,7 +626,7 @@
     </row>
     <row r="8" ht="12.8">
       <c r="A8" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" s="7">
         <v>1113668050704</v>
@@ -648,7 +643,7 @@
     </row>
     <row r="9" ht="12.8">
       <c r="A9" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" s="7">
         <v>1123668013370</v>
@@ -668,7 +663,7 @@
     </row>
     <row r="10" ht="23.95">
       <c r="A10" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B10" s="7">
         <v>1057420008590</v>
@@ -688,7 +683,7 @@
     </row>
     <row r="11" ht="12.8">
       <c r="A11" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" s="7">
         <v>1057421013055</v>
@@ -708,7 +703,7 @@
     </row>
     <row r="12" ht="12.8">
       <c r="A12" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B12" s="7">
         <v>1067203121810</v>
@@ -728,7 +723,7 @@
     </row>
     <row r="13" ht="12.8">
       <c r="A13" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B13" s="7">
         <v>1057421012923</v>
@@ -748,7 +743,7 @@
     </row>
     <row r="14" ht="12.8">
       <c r="A14" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B14" s="7">
         <v>1134704001310</v>
@@ -768,7 +763,7 @@
     </row>
     <row r="15" ht="12.8">
       <c r="A15" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B15" s="7">
         <v>1107232034777</v>
@@ -788,7 +783,7 @@
     </row>
     <row r="16" ht="12.8">
       <c r="A16" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B16" s="7">
         <v>1156658040879</v>
@@ -808,7 +803,7 @@
     </row>
     <row r="17" ht="12.8">
       <c r="A17" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B17" s="7">
         <v>1107456001840</v>
@@ -828,7 +823,7 @@
     </row>
     <row r="18" ht="12.8">
       <c r="A18" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B18" s="7">
         <v>1067438009231</v>
@@ -848,7 +843,7 @@
     </row>
     <row r="19" ht="23.85">
       <c r="A19" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B19" s="7">
         <v>1087232009094</v>
@@ -868,7 +863,7 @@
     </row>
     <row r="20" ht="12.8">
       <c r="A20" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B20" s="7">
         <v>1067203024778</v>
@@ -888,7 +883,7 @@
     </row>
     <row r="21" ht="12.8">
       <c r="A21" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B21" s="7">
         <v>1037200551277</v>
@@ -908,7 +903,7 @@
     </row>
     <row r="22" ht="12.8">
       <c r="A22" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B22" s="7">
         <v>1037200601690</v>
@@ -928,7 +923,7 @@
     </row>
     <row r="23" ht="12.8">
       <c r="A23" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B23" s="7">
         <v>1037200588787</v>
@@ -948,7 +943,7 @@
     </row>
     <row r="24" ht="12.8">
       <c r="A24" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B24" s="7">
         <v>1065032016928</v>
@@ -968,7 +963,7 @@
     </row>
     <row r="25" ht="12.8">
       <c r="A25" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B25" s="7">
         <v>1036602185290</v>
@@ -988,7 +983,7 @@
     </row>
     <row r="26" ht="12.8">
       <c r="A26" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B26" s="7">
         <v>1066142015587</v>
@@ -1008,7 +1003,7 @@
     </row>
     <row r="27" ht="23.85">
       <c r="A27" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B27" s="7">
         <v>1156623000214</v>
@@ -1028,7 +1023,7 @@
     </row>
     <row r="28" ht="12.8">
       <c r="A28" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B28" s="7">
         <v>1096623000429</v>
@@ -1045,7 +1040,7 @@
     </row>
     <row r="29" ht="12.8">
       <c r="A29" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B29" s="7">
         <v>1106623001319</v>
@@ -1065,7 +1060,7 @@
     </row>
     <row r="30" ht="12.8">
       <c r="A30" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B30" s="7">
         <v>1096623001310</v>
@@ -1085,7 +1080,7 @@
     </row>
     <row r="31" ht="12.8">
       <c r="A31" s="7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B31" s="7">
         <v>1096623009163</v>
@@ -1105,7 +1100,7 @@
     </row>
     <row r="32" ht="12.8">
       <c r="A32" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B32" s="7">
         <v>1069623031576</v>
@@ -1125,7 +1120,7 @@
     </row>
     <row r="33" ht="12.8">
       <c r="A33" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B33" s="7">
         <v>1146623006100</v>
@@ -1145,7 +1140,7 @@
     </row>
     <row r="34" ht="12.8">
       <c r="A34" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B34" s="7">
         <v>1096623000286</v>
@@ -1165,7 +1160,7 @@
     </row>
     <row r="35" ht="12.8">
       <c r="A35" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B35" s="7">
         <v>1155050005703</v>
@@ -1185,7 +1180,7 @@
     </row>
     <row r="36" ht="12.8">
       <c r="A36" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B36" s="7">
         <v>1106639001028</v>
@@ -1205,7 +1200,7 @@
     </row>
     <row r="37" ht="12.8">
       <c r="A37" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B37" s="7">
         <v>1106639000973</v>
@@ -1225,7 +1220,7 @@
     </row>
     <row r="38" ht="23.85">
       <c r="A38" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B38" s="7">
         <v>1156658098266</v>
@@ -1245,7 +1240,7 @@
     </row>
     <row r="39" ht="23.95">
       <c r="A39" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B39" s="7">
         <v>1156658098266</v>
@@ -1253,10 +1248,13 @@
       <c r="C39" s="7">
         <v>167</v>
       </c>
+      <c r="D39" s="0">
+        <v>643</v>
+      </c>
     </row>
     <row r="40" ht="23.95">
       <c r="A40" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B40" s="7">
         <v>1156658098266</v>
@@ -1270,7 +1268,7 @@
     </row>
     <row r="41" ht="23.95">
       <c r="A41" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B41" s="7">
         <v>1156658098266</v>
@@ -1284,7 +1282,7 @@
     </row>
     <row r="42" ht="23.95">
       <c r="A42" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B42" s="7">
         <v>1156658098266</v>
@@ -1298,7 +1296,7 @@
     </row>
     <row r="43" ht="12.8">
       <c r="A43" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B43" s="7">
         <v>1156658098266</v>
@@ -1309,7 +1307,7 @@
     </row>
     <row r="44" ht="12.8">
       <c r="A44" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B44" s="7">
         <v>1156658098266</v>
@@ -1320,7 +1318,7 @@
     </row>
     <row r="45" ht="12.8">
       <c r="A45" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B45" s="7">
         <v>1156658098266</v>
@@ -1331,7 +1329,7 @@
     </row>
     <row r="46" ht="12.8">
       <c r="A46" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B46" s="7">
         <v>1156658098266</v>
@@ -1342,7 +1340,7 @@
     </row>
     <row r="47" ht="23.95">
       <c r="A47" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B47" s="7">
         <v>1156658098266</v>
@@ -1356,7 +1354,7 @@
     </row>
     <row r="48" ht="12.8">
       <c r="A48" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B48" s="7">
         <v>1156658098266</v>
@@ -1367,7 +1365,7 @@
     </row>
     <row r="49" ht="23.95">
       <c r="A49" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B49" s="7">
         <v>1156658098266</v>
@@ -1378,7 +1376,7 @@
     </row>
     <row r="50" ht="23.95">
       <c r="A50" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B50" s="7">
         <v>1156658098266</v>
@@ -1389,7 +1387,7 @@
     </row>
     <row r="51" ht="12.8">
       <c r="A51" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B51" s="7">
         <v>1106639000962</v>
@@ -1409,7 +1407,7 @@
     </row>
     <row r="52" ht="12.8">
       <c r="A52" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B52" s="7">
         <v>1106639000896</v>
@@ -1429,7 +1427,7 @@
     </row>
     <row r="53" ht="12.8">
       <c r="A53" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B53" s="7">
         <v>1106639000907</v>
@@ -1449,7 +1447,7 @@
     </row>
     <row r="54" ht="12.8">
       <c r="A54" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B54" s="7">
         <v>1106639000951</v>
@@ -1469,7 +1467,7 @@
     </row>
     <row r="55" ht="12.8">
       <c r="A55" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B55" s="7">
         <v>1146683001420</v>
@@ -1489,7 +1487,7 @@
     </row>
     <row r="56" ht="12.8">
       <c r="A56" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B56" s="7">
         <v>1116671011050</v>
@@ -1509,7 +1507,7 @@
     </row>
     <row r="57" ht="12.8">
       <c r="A57" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B57" s="7">
         <v>1069639010660</v>
@@ -1529,7 +1527,7 @@
     </row>
     <row r="58" ht="12.8">
       <c r="A58" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B58" s="7">
         <v>1027200842811</v>
@@ -1549,7 +1547,7 @@
     </row>
     <row r="59" ht="12.8">
       <c r="A59" s="7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B59" s="7">
         <v>1027200871818</v>
@@ -1569,7 +1567,7 @@
     </row>
     <row r="60" ht="12.8">
       <c r="A60" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B60" s="7">
         <v>1077203003195</v>
@@ -1589,7 +1587,7 @@
     </row>
     <row r="61" ht="12.8">
       <c r="A61" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B61" s="7">
         <v>1087232040466</v>
@@ -1609,7 +1607,7 @@
     </row>
     <row r="62" ht="12.8">
       <c r="A62" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B62" s="7">
         <v>1047200675884</v>
@@ -1629,7 +1627,7 @@
     </row>
     <row r="63" ht="23.85">
       <c r="A63" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B63" s="7">
         <v>1147232021881</v>
@@ -1649,7 +1647,7 @@
     </row>
     <row r="64" ht="12.8">
       <c r="A64" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B64" s="7">
         <v>1077200004122</v>
@@ -1669,7 +1667,7 @@
     </row>
     <row r="65" ht="12.8">
       <c r="A65" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B65" s="7">
         <v>1147232017580</v>
@@ -1689,7 +1687,7 @@
     </row>
     <row r="66" ht="12.8">
       <c r="A66" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B66" s="7">
         <v>1087232040697</v>
@@ -1709,7 +1707,7 @@
     </row>
     <row r="67" ht="12.8">
       <c r="A67" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B67" s="7">
         <v>1116674014270</v>
@@ -1729,7 +1727,7 @@
     </row>
     <row r="68" ht="12.8">
       <c r="A68" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B68" s="7">
         <v>1141828000710</v>
@@ -1746,7 +1744,7 @@
     </row>
     <row r="69" ht="12.8">
       <c r="A69" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B69" s="7">
         <v>1046601020157</v>
@@ -1766,7 +1764,7 @@
     </row>
     <row r="70" ht="12.8">
       <c r="A70" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B70" s="7">
         <v>1086639001481</v>
@@ -1786,7 +1784,7 @@
     </row>
     <row r="71" ht="12.8">
       <c r="A71" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B71" s="7">
         <v>1147232040196</v>
@@ -1806,7 +1804,7 @@
     </row>
     <row r="72" ht="12.8">
       <c r="A72" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B72" s="7">
         <v>1167232056551</v>
@@ -1826,7 +1824,7 @@
     </row>
     <row r="73" ht="12.8">
       <c r="A73" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B73" s="7">
         <v>1157232026137</v>
@@ -1843,7 +1841,7 @@
     </row>
     <row r="74" ht="12.8">
       <c r="A74" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B74" s="7">
         <v>1107232017595</v>
@@ -1863,7 +1861,7 @@
     </row>
     <row r="75" ht="12.8">
       <c r="A75" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B75" s="7">
         <v>1027200836464</v>
@@ -1883,7 +1881,7 @@
     </row>
     <row r="76" ht="12.8">
       <c r="A76" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B76" s="7">
         <v>1069633012008</v>
@@ -1900,7 +1898,7 @@
     </row>
     <row r="77" ht="12.8">
       <c r="A77" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B77" s="7">
         <v>1096607000159</v>
@@ -1917,7 +1915,7 @@
     </row>
     <row r="78" ht="12.8">
       <c r="A78" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B78" s="7">
         <v>1146623005913</v>
@@ -1937,7 +1935,7 @@
     </row>
     <row r="79" ht="12.8">
       <c r="A79" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B79" s="7">
         <v>1026600785430</v>
@@ -1957,7 +1955,7 @@
     </row>
     <row r="80" ht="12.8">
       <c r="A80" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B80" s="7">
         <v>1152036004625</v>
@@ -1977,7 +1975,7 @@
     </row>
     <row r="81" ht="12.8">
       <c r="A81" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B81" s="7">
         <v>1107232017089</v>
@@ -1997,7 +1995,7 @@
     </row>
     <row r="82" ht="12.8">
       <c r="A82" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B82" s="7">
         <v>1076633000762</v>
@@ -2014,7 +2012,7 @@
     </row>
     <row r="83" ht="12.8">
       <c r="A83" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B83" s="7">
         <v>1057200754346</v>
@@ -2034,7 +2032,7 @@
     </row>
     <row r="84" ht="12.8">
       <c r="A84" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B84" s="7">
         <v>1047200601766</v>
@@ -2068,7 +2066,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G208"/>
+  <dimension ref="A1:G209"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
@@ -4635,10 +4633,10 @@
         <v>7249</v>
       </c>
       <c r="E128" s="0">
-        <v>2125</v>
+        <v>3468</v>
       </c>
       <c r="F128" s="0">
-        <v>731</v>
+        <v>831</v>
       </c>
       <c r="G128" s="0" t="s">
         <v>15</v>
@@ -5595,10 +5593,10 @@
         <v>2771</v>
       </c>
       <c r="E176" s="0">
-        <v>388</v>
+        <v>702</v>
       </c>
       <c r="F176" s="0">
-        <v>241</v>
+        <v>427</v>
       </c>
       <c r="G176" s="0" t="s">
         <v>18</v>
@@ -5669,19 +5667,19 @@
         <v>614</v>
       </c>
       <c r="B180" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D180" s="0">
         <v>2005</v>
       </c>
       <c r="E180" s="0">
-        <v>823</v>
+        <v>1273</v>
       </c>
       <c r="F180" s="0">
-        <v>480</v>
+        <v>732</v>
       </c>
       <c r="G180" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="181">
@@ -5761,7 +5759,7 @@
         <v>0</v>
       </c>
       <c r="G184" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="185">
@@ -5821,7 +5819,7 @@
         <v>0</v>
       </c>
       <c r="G187" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="188">
@@ -6032,16 +6030,16 @@
         <v>1</v>
       </c>
       <c r="D198" s="0">
-        <v>0</v>
+        <v>35226</v>
       </c>
       <c r="E198" s="0">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="F198" s="0">
         <v>0</v>
       </c>
       <c r="G198" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="199">
@@ -6049,7 +6047,7 @@
         <v>633</v>
       </c>
       <c r="B199" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D199" s="0">
         <v>4449</v>
@@ -6058,10 +6056,10 @@
         <v>0</v>
       </c>
       <c r="F199" s="0">
-        <v>0</v>
+        <v>4449</v>
       </c>
       <c r="G199" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="200">
@@ -6069,7 +6067,7 @@
         <v>634</v>
       </c>
       <c r="B200" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D200" s="0">
         <v>4449</v>
@@ -6078,10 +6076,10 @@
         <v>0</v>
       </c>
       <c r="F200" s="0">
-        <v>0</v>
+        <v>4449</v>
       </c>
       <c r="G200" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="201">
@@ -6109,7 +6107,7 @@
         <v>636</v>
       </c>
       <c r="B202" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D202" s="0">
         <v>2977</v>
@@ -6118,10 +6116,10 @@
         <v>0</v>
       </c>
       <c r="F202" s="0">
-        <v>0</v>
+        <v>2977</v>
       </c>
       <c r="G202" s="0" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="203">
@@ -6181,7 +6179,7 @@
         <v>0</v>
       </c>
       <c r="G205" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="206">
@@ -6192,16 +6190,16 @@
         <v>1</v>
       </c>
       <c r="D206" s="0">
-        <v>0</v>
+        <v>28279</v>
       </c>
       <c r="E206" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F206" s="0">
-        <v>0</v>
+        <v>5732</v>
       </c>
       <c r="G206" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="207">
@@ -6209,19 +6207,19 @@
         <v>641</v>
       </c>
       <c r="B207" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D207" s="0">
-        <v>0</v>
+        <v>11690</v>
       </c>
       <c r="E207" s="0">
         <v>0</v>
       </c>
       <c r="F207" s="0">
-        <v>0</v>
+        <v>11690</v>
       </c>
       <c r="G207" s="0" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="208">
@@ -6242,6 +6240,14 @@
       </c>
       <c r="G208" s="0" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="0">
+        <v>643</v>
+      </c>
+      <c r="B209" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>